<commit_message>
INPUT SUCCESSFULL, compare right wrong start
</commit_message>
<xml_diff>
--- a/QuizQuestions final.xlsx
+++ b/QuizQuestions final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2024_SR_12IT1\Programming\AS91897QuizGameGUI_ShuklaMahit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A54A5A-EED2-42DB-864F-61890074071F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4329E2A-CE1E-42F7-B0D6-9C181957DCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Question</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Gravity</t>
   </si>
   <si>
-    <t>π</t>
-  </si>
-  <si>
     <t>Urea cycle</t>
   </si>
   <si>
@@ -168,6 +165,21 @@
   </si>
   <si>
     <t>Pancreas</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -503,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +529,7 @@
     <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +545,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -550,25 +565,31 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -584,8 +605,11 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -601,8 +625,11 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -618,8 +645,11 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -635,8 +665,11 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -652,8 +685,11 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -669,8 +705,11 @@
       <c r="E9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -680,45 +719,51 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
+      <c r="D10" s="2">
+        <v>2.43562235</v>
       </c>
       <c r="E10">
         <v>-23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>